<commit_message>
supp and use tables 2014
</commit_message>
<xml_diff>
--- a/outdata/test2014.xlsx
+++ b/outdata/test2014.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pttry.sharepoint.com/sites/KT_SAlueellinentilinpitojrjestelm/Shared Documents/General/koodi/alta/outdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janne.huovari\Pellervon Taloustutkimus PTT ry\KT_S Alueellinen tilinpito - Documents\General\koodi\alta\outdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_FAEFE1C26CE0057602BD06938563BEB41421EB3D" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{217C1239-58D5-42FA-8BED-9E36FEFFC81B}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_FAEFE1C26CE0057602BD06938563BEB41421EB3D" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{DA9C9F81-1F19-447C-AAEA-1A9FB1ED4E7E}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11205" yWindow="0" windowWidth="17400" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uusimaa" sheetId="1" r:id="rId1"/>
@@ -640,15 +640,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ32"/>
+  <dimension ref="A1:AK32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AH32" sqref="AH32"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AK3" sqref="AK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -749,7 +749,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -847,7 +847,7 @@
         <v>220.890869140625</v>
       </c>
       <c r="AG2">
-        <v>414.97763061523438</v>
+        <v>414.97763061523398</v>
       </c>
       <c r="AH2">
         <v>635.8685302734375</v>
@@ -859,8 +859,12 @@
         <f>AH2+AI2</f>
         <v>1677.8685302734375</v>
       </c>
+      <c r="AK2">
+        <f>AG2-70</f>
+        <v>344.97763061523398</v>
+      </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -964,7 +968,7 @@
         <v>318.8587646484375</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
@@ -1068,7 +1072,7 @@
         <v>4068.97021484375</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
@@ -1172,7 +1176,7 @@
         <v>4600.85791015625</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
@@ -1276,7 +1280,7 @@
         <v>1546.452392578125</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
@@ -1380,7 +1384,7 @@
         <v>297.12039184570313</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>39</v>
       </c>
@@ -1484,7 +1488,7 @@
         <v>2127.958251953125</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
@@ -1588,7 +1592,7 @@
         <v>15372.033203125</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -1692,7 +1696,7 @@
         <v>863.11767578125</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -1796,7 +1800,7 @@
         <v>2708.572998046875</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -1900,7 +1904,7 @@
         <v>6648.2353515625</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -2004,7 +2008,7 @@
         <v>3433.125732421875</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -2108,7 +2112,7 @@
         <v>1668.842041015625</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -2212,7 +2216,7 @@
         <v>2331.84228515625</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
@@ -3867,7 +3871,7 @@
         <v>43.653896331787109</v>
       </c>
       <c r="AF31">
-        <v>43.653896331787109</v>
+        <v>43.653896331787102</v>
       </c>
       <c r="AG31">
         <v>0</v>
@@ -64070,18 +64074,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -64250,26 +64254,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16884085-D5F6-4A1E-AE2D-9EE2821F727B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B2821F-8C01-4796-BB56-35465F4B5EC5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f6d38416-0c3a-40f5-a98e-64d30975dddf"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="5d070ba9-5dd2-4ec6-9127-c85124792d21"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B2821F-8C01-4796-BB56-35465F4B5EC5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16884085-D5F6-4A1E-AE2D-9EE2821F727B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="5d070ba9-5dd2-4ec6-9127-c85124792d21"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f6d38416-0c3a-40f5-a98e-64d30975dddf"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>